<commit_message>
Change Dutch descriptions into English
</commit_message>
<xml_diff>
--- a/data/sdh-ratio.xlsx
+++ b/data/sdh-ratio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanvanderzwaard/Projects/research/myoglobin/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanvanderzwaard/Projects/research/2022-myoglobin/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA98E3B-3A34-E443-9D93-21F1E01B3BCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF0C881-AC53-5E4A-86A5-0128DB6E7404}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="2800" windowWidth="27840" windowHeight="16740" xr2:uid="{CA26C2CA-5023-694E-BAFC-9E9CDC5280E2}"/>
   </bookViews>
@@ -70,9 +70,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
-    <t>Ppnummer</t>
-  </si>
-  <si>
     <t>SF-PP01</t>
   </si>
   <si>
@@ -220,22 +217,25 @@
     <t>PS-PP000</t>
   </si>
   <si>
-    <t>SF</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>Groep: 1= wielrenners</t>
-  </si>
-  <si>
-    <t>Groep: 2=sportvasters</t>
-  </si>
-  <si>
-    <t>SDH I / II</t>
-  </si>
-  <si>
-    <t>Groep</t>
+    <t>PP-number</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Ratio SDH I / II</t>
+  </si>
+  <si>
+    <t>controls</t>
+  </si>
+  <si>
+    <t>cyclists</t>
+  </si>
+  <si>
+    <t>Groep: 1= cyclists</t>
+  </si>
+  <si>
+    <t>Groep: 2=controls</t>
   </si>
 </sst>
 </file>
@@ -766,7 +766,7 @@
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,18 +780,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="11">
         <v>2</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="12">
         <v>2</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="12">
         <v>2</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="12">
         <v>2</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="12">
         <v>2</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="12">
         <v>2</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="12">
         <v>2</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="12">
         <v>2</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="12">
         <v>2</v>
@@ -890,7 +890,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="12">
         <v>2</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="12">
         <v>2</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="12">
         <v>2</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="12">
         <v>2</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="12">
         <v>2</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="12">
         <v>2</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="12">
         <v>2</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="12">
         <v>2</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="12">
         <v>2</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="12">
         <v>2</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="22" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="13">
         <v>2</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="12">
         <v>1</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="14">
         <v>1</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="14">
         <v>1</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="14">
         <v>1</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="14">
         <v>1</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="14">
         <v>1</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="14">
         <v>1</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="14">
         <v>1</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="14">
         <v>1</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="14">
         <v>1</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="14">
         <v>1</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="14">
         <v>1</v>
@@ -1150,7 +1150,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="14">
         <v>1</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="14">
         <v>1</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="14">
         <v>1</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="14">
         <v>1</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="14">
         <v>1</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="14">
         <v>1</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="14">
         <v>1</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="14">
         <v>1</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="14">
         <v>1</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="14">
         <v>1</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="14">
         <v>1</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="14">
         <v>1</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="14">
         <v>1</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="14">
         <v>1</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="14">
         <v>1</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="15">
         <v>1</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="8" t="str">
@@ -1339,7 +1339,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="8" t="str">
@@ -1353,12 +1353,12 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>